<commit_message>
added covid to the mainframe
and some nfts too
</commit_message>
<xml_diff>
--- a/Trabalho_Prático_1/table.xlsx
+++ b/Trabalho_Prático_1/table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\35192\Documents\UNI\3rd Year\2nd Semester\MULT\Práticas\Trabalho_Prático_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADE4DF9C-571E-461E-A1C2-DA9FEA2097DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1101CDA3-01C3-4FF6-9F25-BE6F81D2B1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{F6381695-21DE-4986-B177-5A87DA81EF96}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Image</t>
   </si>
@@ -46,7 +46,79 @@
     <t>Compressed Size</t>
   </si>
   <si>
-    <t>Compress Ratio</t>
+    <t>Compression Ratio</t>
+  </si>
+  <si>
+    <t>348 KB</t>
+  </si>
+  <si>
+    <t>barn_mountains.bmp</t>
+  </si>
+  <si>
+    <t>logo.bmp</t>
+  </si>
+  <si>
+    <t>411 KB</t>
+  </si>
+  <si>
+    <t>peppers.bmp</t>
+  </si>
+  <si>
+    <t>576 KB</t>
+  </si>
+  <si>
+    <t>19,7 KB</t>
+  </si>
+  <si>
+    <t>32,6 KB</t>
+  </si>
+  <si>
+    <t>60,6 KB</t>
+  </si>
+  <si>
+    <t>6,07 KB</t>
+  </si>
+  <si>
+    <t>8,15 KB</t>
+  </si>
+  <si>
+    <t>12,9 KB</t>
+  </si>
+  <si>
+    <t>15,7 KB</t>
+  </si>
+  <si>
+    <t>26,3 KB</t>
+  </si>
+  <si>
+    <t>56,0 KB</t>
+  </si>
+  <si>
+    <t>17,66 : 1</t>
+  </si>
+  <si>
+    <t>10,67 : 1</t>
+  </si>
+  <si>
+    <t>5,74 : 1</t>
+  </si>
+  <si>
+    <t>50,42 : 1</t>
+  </si>
+  <si>
+    <t>31,86 : 1</t>
+  </si>
+  <si>
+    <t>67,71 : 1</t>
+  </si>
+  <si>
+    <t>36,68 : 1</t>
+  </si>
+  <si>
+    <t>21,9 : 1</t>
+  </si>
+  <si>
+    <t>10,28 : 1</t>
   </si>
 </sst>
 </file>
@@ -70,12 +142,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -131,27 +221,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,138 +563,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26CC8BB6-C879-4D1D-8D58-4E790FDEE638}">
-  <dimension ref="B3:N10"/>
+  <dimension ref="B3:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="1" t="s">
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="3">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="2">
         <v>25</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>50</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>75</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>25</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>50</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <v>75</v>
       </c>
+      <c r="N4" s="10"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="2"/>
+      <c r="B5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="2"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="2"/>
+      <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="2"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="2"/>
-      <c r="N9" s="7"/>
+      <c r="B9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="1"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="2"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N11" s="1"/>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="B7:C8"/>
+    <mergeCell ref="B9:C10"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="D9:E10"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
     <mergeCell ref="K9:K10"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="I5:I6"/>
@@ -605,27 +780,6 @@
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:K8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="B5:C6"/>
-    <mergeCell ref="B7:C8"/>
-    <mergeCell ref="B9:C10"/>
-    <mergeCell ref="D5:E6"/>
-    <mergeCell ref="D7:E8"/>
-    <mergeCell ref="D9:E10"/>
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="I3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>